<commit_message>
added id to platform address
</commit_message>
<xml_diff>
--- a/xBee_to_Platform.xlsx
+++ b/xBee_to_Platform.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amy\Google Drive\2015-2016 NGCP\Comms\NGCP Comms 2015-2016\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="8340"/>
   </bookViews>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
   <si>
     <t>last 4 digits</t>
   </si>
@@ -132,6 +127,9 @@
   </si>
   <si>
     <t>ROV Alternate</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -257,7 +255,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -292,7 +290,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -501,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,12 +512,12 @@
     <col min="3" max="3" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -529,8 +527,11 @@
       <c r="C2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -540,8 +541,11 @@
       <c r="C3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -551,8 +555,11 @@
       <c r="C4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -562,8 +569,11 @@
       <c r="C5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -573,16 +583,22 @@
       <c r="C6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -592,13 +608,24 @@
       <c r="C8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -608,8 +635,11 @@
       <c r="C11" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -619,8 +649,11 @@
       <c r="C12" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -630,8 +663,11 @@
       <c r="C13" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -641,8 +677,11 @@
       <c r="C14" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -652,8 +691,11 @@
       <c r="C15" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>31</v>
       </c>
@@ -663,8 +705,11 @@
       <c r="C16" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>34</v>
       </c>
@@ -673,6 +718,9 @@
       </c>
       <c r="C17" t="s">
         <v>36</v>
+      </c>
+      <c r="D17">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>